<commit_message>
finalized interim presentation and updated gantt chart
</commit_message>
<xml_diff>
--- a/FinalYearProject/ganttChart.xlsx
+++ b/FinalYearProject/ganttChart.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22228"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Year4\FinalYearProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Year4\FYP\FinalYearProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB265C99-E4AD-4E6F-98BA-FC13BA66530B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC6B1C5C-3043-4856-8134-4E98605E7A07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1039,17 +1039,28 @@
   </sheetPr>
   <dimension ref="A1:BO19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="AW21" sqref="AW21"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="60" zoomScaleNormal="60" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="AV12" sqref="AV12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2.625" customWidth="1"/>
-    <col min="2" max="2" width="27.375" style="2" customWidth="1"/>
-    <col min="3" max="6" width="11.625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15.625" style="4" customWidth="1"/>
-    <col min="8" max="27" width="2.75" style="1"/>
+    <col min="2" max="2" width="57.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.875" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2.5" style="1" customWidth="1"/>
+    <col min="9" max="15" width="2.75" style="1"/>
+    <col min="16" max="16" width="2.75" style="1" customWidth="1"/>
+    <col min="17" max="17" width="3.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="3.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="26" width="3.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="3.75" bestFit="1" customWidth="1"/>
+    <col min="29" max="35" width="4" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="2.75" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1073,7 +1084,7 @@
         <v>4</v>
       </c>
       <c r="H2" s="11">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="J2" s="12"/>
       <c r="K2" s="33" t="s">
@@ -1687,7 +1698,7 @@
         <v>5</v>
       </c>
       <c r="G13" s="21">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="H13" s="22"/>
       <c r="I13" s="22"/>
@@ -1728,10 +1739,14 @@
       <c r="D14" s="20">
         <v>1</v>
       </c>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
+      <c r="E14" s="20">
+        <v>11</v>
+      </c>
+      <c r="F14" s="20">
+        <v>1</v>
+      </c>
       <c r="G14" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" s="22"/>
       <c r="I14" s="22"/>

</xml_diff>

<commit_message>
created template popup windowns for join and create classroom sections
</commit_message>
<xml_diff>
--- a/FinalYearProject/ganttChart.xlsx
+++ b/FinalYearProject/ganttChart.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22325"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Year4\FYP\FinalYearProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC6B1C5C-3043-4856-8134-4E98605E7A07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A4F5441-A402-4320-8A51-60C974990877}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1040,7 +1040,7 @@
   <dimension ref="A1:BO19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="60" zoomScaleNormal="60" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="AV12" sqref="AV12"/>
+      <selection activeCell="AC15" sqref="AC15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1084,7 +1084,7 @@
         <v>4</v>
       </c>
       <c r="H2" s="11">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="J2" s="12"/>
       <c r="K2" s="33" t="s">

</xml_diff>

<commit_message>
more work on dissertation
</commit_message>
<xml_diff>
--- a/FinalYearProject/ganttChart.xlsx
+++ b/FinalYearProject/ganttChart.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Year4\FYP\FinalYearProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A4F5441-A402-4320-8A51-60C974990877}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9D24CFD-D559-43C1-B351-8CDD27EAB6E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1039,8 +1039,8 @@
   </sheetPr>
   <dimension ref="A1:BO19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="60" zoomScaleNormal="60" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="AC15" sqref="AC15"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="AG6" sqref="AG6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1051,8 +1051,8 @@
     <col min="4" max="4" width="12.125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.75" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.875" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="2.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="20.625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.375" style="1" customWidth="1"/>
     <col min="9" max="15" width="2.75" style="1"/>
     <col min="16" max="16" width="2.75" style="1" customWidth="1"/>
     <col min="17" max="17" width="3.75" style="1" bestFit="1" customWidth="1"/>
@@ -1084,7 +1084,7 @@
         <v>4</v>
       </c>
       <c r="H2" s="11">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="J2" s="12"/>
       <c r="K2" s="33" t="s">
@@ -1787,10 +1787,14 @@
       <c r="D15" s="20">
         <v>11</v>
       </c>
-      <c r="E15" s="20"/>
-      <c r="F15" s="20"/>
+      <c r="E15" s="20">
+        <v>12</v>
+      </c>
+      <c r="F15" s="20">
+        <v>12</v>
+      </c>
       <c r="G15" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" s="22"/>
       <c r="I15" s="22"/>
@@ -1831,10 +1835,14 @@
       <c r="D16" s="20">
         <v>15</v>
       </c>
-      <c r="E16" s="20"/>
-      <c r="F16" s="20"/>
+      <c r="E16" s="20">
+        <v>12</v>
+      </c>
+      <c r="F16" s="20">
+        <v>15</v>
+      </c>
       <c r="G16" s="21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="H16" s="22"/>
       <c r="I16" s="22"/>
@@ -1875,10 +1883,14 @@
       <c r="D17" s="20">
         <v>3</v>
       </c>
-      <c r="E17" s="20"/>
-      <c r="F17" s="20"/>
+      <c r="E17" s="20">
+        <v>24</v>
+      </c>
+      <c r="F17" s="20">
+        <v>2</v>
+      </c>
       <c r="G17" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H17" s="22"/>
       <c r="I17" s="22"/>
@@ -1919,10 +1931,14 @@
       <c r="D18" s="20">
         <v>3</v>
       </c>
-      <c r="E18" s="20"/>
-      <c r="F18" s="20"/>
+      <c r="E18" s="20">
+        <v>24</v>
+      </c>
+      <c r="F18" s="20">
+        <v>2</v>
+      </c>
       <c r="G18" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H18" s="22"/>
       <c r="I18" s="22"/>

</xml_diff>